<commit_message>
Se agrega el archivo sql para la creacion de la DB
</commit_message>
<xml_diff>
--- a/sql/normalizacion_biblioteca.xlsx
+++ b/sql/normalizacion_biblioteca.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compi\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reyap\Desktop\Biblioteca-SQL\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633F09F-8CDA-4205-A262-F6F6427E263B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8EB7CE-DA4C-4532-BA59-D66BCD4A47E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00C2CB17-EDF4-4994-8FF5-2A81667E2E86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00C2CB17-EDF4-4994-8FF5-2A81667E2E86}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +241,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,7 +265,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,13 +272,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14B3DC3-02C9-4910-9155-8484B1C9022F}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57:M57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,35 +635,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -673,7 +681,7 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>41744</v>
       </c>
     </row>
@@ -693,7 +701,7 @@
       <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>41746</v>
       </c>
     </row>
@@ -713,7 +721,7 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>41745</v>
       </c>
     </row>
@@ -733,7 +741,7 @@
       <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>41749</v>
       </c>
     </row>
@@ -753,60 +761,60 @@
       <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>41747</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -832,7 +840,7 @@
       <c r="G12" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>41744</v>
       </c>
     </row>
@@ -858,7 +866,7 @@
       <c r="G13" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>41746</v>
       </c>
     </row>
@@ -884,7 +892,7 @@
       <c r="G14" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>41745</v>
       </c>
     </row>
@@ -910,7 +918,7 @@
       <c r="G15" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>41749</v>
       </c>
     </row>
@@ -936,63 +944,63 @@
       <c r="G16" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>41747</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="E19" s="6" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="E19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="F20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="3">
-        <v>1</v>
-      </c>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C21">
@@ -1016,15 +1024,15 @@
       <c r="J21" t="s">
         <v>33</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K21" s="1">
         <v>41744</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>2</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C22">
@@ -1048,15 +1056,15 @@
       <c r="J22" t="s">
         <v>34</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="1">
         <v>41746</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>3</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C23">
@@ -1080,15 +1088,15 @@
       <c r="J23" t="s">
         <v>35</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="1">
         <v>41745</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>4</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C24">
@@ -1112,15 +1120,15 @@
       <c r="J24" t="s">
         <v>36</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="1">
         <v>41749</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>5</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C25">
@@ -1144,15 +1152,15 @@
       <c r="J25" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>41747</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>1</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="A26" s="2">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C26">
@@ -1160,39 +1168,38 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="D31" s="6" t="s">
+      <c r="B31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="G31" s="6" t="s">
+      <c r="E31" s="4"/>
+      <c r="G31" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="6" t="s">
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="L31" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -1201,35 +1208,35 @@
       <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" s="3" t="s">
+      <c r="H32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3" t="s">
+      <c r="K32" s="2"/>
+      <c r="L32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M32" s="3" t="s">
+      <c r="M32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N32" s="3" t="s">
+      <c r="N32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="O32" s="3" t="s">
+      <c r="O32" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1240,10 +1247,10 @@
       <c r="B33">
         <v>1001</v>
       </c>
-      <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G33">
@@ -1255,7 +1262,7 @@
       <c r="I33" t="s">
         <v>15</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="1">
         <v>41744</v>
       </c>
       <c r="L33">
@@ -1278,10 +1285,10 @@
       <c r="B34">
         <v>1005</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>2</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G34">
@@ -1293,7 +1300,7 @@
       <c r="I34" t="s">
         <v>16</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
         <v>41746</v>
       </c>
       <c r="L34">
@@ -1316,10 +1323,10 @@
       <c r="B35">
         <v>1004</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>3</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G35">
@@ -1331,7 +1338,7 @@
       <c r="I35" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="1">
         <v>41745</v>
       </c>
       <c r="L35">
@@ -1354,10 +1361,10 @@
       <c r="B36">
         <v>1006</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>4</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G36">
@@ -1369,7 +1376,7 @@
       <c r="I36" t="s">
         <v>17</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="1">
         <v>41749</v>
       </c>
       <c r="L36">
@@ -1392,10 +1399,10 @@
       <c r="B37">
         <v>1006</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>5</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G37">
@@ -1407,7 +1414,7 @@
       <c r="I37" t="s">
         <v>15</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="1">
         <v>41747</v>
       </c>
     </row>
@@ -1418,20 +1425,20 @@
       <c r="B38">
         <v>1007</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="4"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L39" s="6" t="s">
+      <c r="L39" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M39" s="6"/>
+      <c r="M39" s="4"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L40" s="3" t="s">
+      <c r="L40" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M40" s="3" t="s">
+      <c r="M40" s="2" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1476,40 +1483,39 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="D49" s="6" t="s">
+      <c r="B49" s="7"/>
+      <c r="D49" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="6"/>
-      <c r="G49" s="6" t="s">
+      <c r="E49" s="7"/>
+      <c r="G49" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="6" t="s">
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="K49" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L49" s="6"/>
-      <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -1518,32 +1524,32 @@
       <c r="B50" t="s">
         <v>44</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I50" s="3" t="s">
+      <c r="H50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3" t="s">
+      <c r="J50" s="2"/>
+      <c r="K50" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L50" s="3" t="s">
+      <c r="L50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M50" s="3" t="s">
+      <c r="M50" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N50" s="3" t="s">
+      <c r="N50" s="2" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1554,10 +1560,10 @@
       <c r="B51">
         <v>1001</v>
       </c>
-      <c r="D51" s="3">
-        <v>1</v>
-      </c>
-      <c r="E51" s="4" t="s">
+      <c r="D51" s="2">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G51">
@@ -1589,10 +1595,10 @@
       <c r="B52">
         <v>1005</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <v>2</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="E52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G52">
@@ -1624,10 +1630,10 @@
       <c r="B53">
         <v>1004</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2">
         <v>3</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G53">
@@ -1659,10 +1665,10 @@
       <c r="B54">
         <v>1006</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="2">
         <v>4</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G54">
@@ -1694,10 +1700,10 @@
       <c r="B55">
         <v>1006</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="2">
         <v>5</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G55">
@@ -1717,19 +1723,19 @@
       <c r="B56">
         <v>1007</v>
       </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G57" s="6" t="s">
+      <c r="G57" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H57" s="6"/>
-      <c r="K57" s="6" t="s">
+      <c r="H57" s="7"/>
+      <c r="K57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G58" t="s">
@@ -1738,10 +1744,10 @@
       <c r="H58" t="s">
         <v>50</v>
       </c>
-      <c r="K58" s="3" t="s">
+      <c r="K58" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L58" s="3" t="s">
+      <c r="L58" s="2" t="s">
         <v>53</v>
       </c>
       <c r="M58" t="s">
@@ -1761,7 +1767,7 @@
       <c r="L59">
         <v>1</v>
       </c>
-      <c r="M59" s="2">
+      <c r="M59" s="1">
         <v>41744</v>
       </c>
     </row>
@@ -1778,7 +1784,7 @@
       <c r="L60">
         <v>2</v>
       </c>
-      <c r="M60" s="2">
+      <c r="M60" s="1">
         <v>41746</v>
       </c>
     </row>
@@ -1795,7 +1801,7 @@
       <c r="L61">
         <v>3</v>
       </c>
-      <c r="M61" s="2">
+      <c r="M61" s="1">
         <v>41745</v>
       </c>
     </row>
@@ -1806,7 +1812,7 @@
       <c r="L62">
         <v>4</v>
       </c>
-      <c r="M62" s="2">
+      <c r="M62" s="1">
         <v>41749</v>
       </c>
     </row>
@@ -1817,12 +1823,22 @@
       <c r="L63">
         <v>1</v>
       </c>
-      <c r="M63" s="2">
+      <c r="M63" s="1">
         <v>41747</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="E19:K19"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="L31:O31"/>
     <mergeCell ref="G57:H57"/>
     <mergeCell ref="G49:I49"/>
     <mergeCell ref="K57:M57"/>
@@ -1831,16 +1847,6 @@
     <mergeCell ref="A47:J47"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="E19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>